<commit_message>
transportation and waste disposal pages (without data linking)
</commit_message>
<xml_diff>
--- a/ProductsDataCleaning.xlsx
+++ b/ProductsDataCleaning.xlsx
@@ -1789,8 +1789,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1799,11 +1801,13 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2135,7 +2139,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:W51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>

<commit_message>
Disposal Table View data populated
</commit_message>
<xml_diff>
--- a/ProductsDataCleaning.xlsx
+++ b/ProductsDataCleaning.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="574">
   <si>
     <t>code</t>
   </si>
@@ -93,9 +93,6 @@
     <t>http://world-en.openfoodfacts.org/product/0000000024600/filet-de-boeuf</t>
   </si>
   <si>
-    <t>Filet de bœuf</t>
-  </si>
-  <si>
     <t>2.46 kg</t>
   </si>
   <si>
@@ -165,15 +162,9 @@
     <t>http://world-en.openfoodfacts.org/product/0000005200016/lentilles-vertes-bertrand-lejeune</t>
   </si>
   <si>
-    <t xml:space="preserve">lentilles vertes </t>
-  </si>
-  <si>
     <t xml:space="preserve">1 kg </t>
   </si>
   <si>
-    <t>Sachet plastique</t>
-  </si>
-  <si>
     <t>sachet-plastique</t>
   </si>
   <si>
@@ -318,9 +309,6 @@
     <t>http://world-en.openfoodfacts.org/product/0000012345878/%E0%B9%80%E0%B8%A5%E0%B9%87%E0%B8%9A%E0%B8%A1%E0%B8%B7%E0%B8%AD%E0%B8%99%E0%B8%B2%E0%B8%87-%E0%B8%95%E0%B8%B5%E0%B8%99%E0%B9%84%E0%B8%81%E0%B9%88-thai-import</t>
   </si>
   <si>
-    <t>เล็บมือนาง (ตีนไก่ )</t>
-  </si>
-  <si>
     <t>chicken feet</t>
   </si>
   <si>
@@ -354,9 +342,6 @@
     <t>http://world-en.openfoodfacts.org/product/0000027533024/luxury-christmas-pudding-asda</t>
   </si>
   <si>
-    <t>Luxury Christmas Pudding</t>
-  </si>
-  <si>
     <t>454g</t>
   </si>
   <si>
@@ -438,9 +423,6 @@
     <t>http://world-en.openfoodfacts.org/product/0000040608754/pepsi-nouveau-gout</t>
   </si>
   <si>
-    <t>Pepsi, Nouveau goût !</t>
-  </si>
-  <si>
     <t>Boisson gazeuse rafraîchissante aux extraits naturels de végétaux</t>
   </si>
   <si>
@@ -528,9 +510,6 @@
     <t>300 g (neto)</t>
   </si>
   <si>
-    <t>Bote de plástico</t>
-  </si>
-  <si>
     <t>bote-de-plastico</t>
   </si>
   <si>
@@ -1741,6 +1720,30 @@
   </si>
   <si>
     <t>green</t>
+  </si>
+  <si>
+    <t>Beef filet</t>
+  </si>
+  <si>
+    <t>Sachet plastic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lentilles </t>
+  </si>
+  <si>
+    <t>Luxury Christmas Pudding 454g</t>
+  </si>
+  <si>
+    <t>Luxury Christmas Pudding 907g</t>
+  </si>
+  <si>
+    <t>Plastic bottle</t>
+  </si>
+  <si>
+    <t>Pepsi 33cl</t>
+  </si>
+  <si>
+    <t>Pepsi 15cl</t>
   </si>
 </sst>
 </file>
@@ -1772,12 +1775,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1789,7 +1798,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1797,17 +1806,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2140,7 +2154,7 @@
   <dimension ref="A1:W51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:W51"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2216,7 +2230,7 @@
         <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -2226,38 +2240,38 @@
       <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="E2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
         <v>28</v>
       </c>
-      <c r="S2" t="s">
-        <v>28</v>
-      </c>
-      <c r="T2" t="s">
-        <v>26</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>29</v>
-      </c>
-      <c r="V2" t="s">
-        <v>30</v>
       </c>
       <c r="W2">
         <v>0</v>
@@ -2268,55 +2282,55 @@
         <v>1071894</v>
       </c>
       <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>33</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>34</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>35</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" t="s">
         <v>36</v>
       </c>
-      <c r="J3" t="s">
+      <c r="M3" t="s">
         <v>38</v>
       </c>
-      <c r="K3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>39</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>40</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>41</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>42</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>43</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>44</v>
-      </c>
-      <c r="V3" t="s">
-        <v>45</v>
       </c>
       <c r="W3">
         <v>0</v>
@@ -2327,49 +2341,49 @@
         <v>5200016</v>
       </c>
       <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="E4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
+        <v>567</v>
+      </c>
+      <c r="G4" t="s">
         <v>47</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>48</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>49</v>
       </c>
-      <c r="G4" t="s">
+      <c r="L4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" t="s">
         <v>50</v>
       </c>
-      <c r="H4" t="s">
+      <c r="P4" t="s">
         <v>51</v>
       </c>
-      <c r="I4" t="s">
+      <c r="R4" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" t="s">
         <v>52</v>
       </c>
-      <c r="L4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="T4" t="s">
+        <v>42</v>
+      </c>
+      <c r="U4" t="s">
         <v>53</v>
       </c>
-      <c r="P4" t="s">
+      <c r="V4" t="s">
         <v>54</v>
-      </c>
-      <c r="R4" t="s">
-        <v>41</v>
-      </c>
-      <c r="S4" t="s">
-        <v>55</v>
-      </c>
-      <c r="T4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U4" t="s">
-        <v>56</v>
-      </c>
-      <c r="V4" t="s">
-        <v>57</v>
       </c>
       <c r="W4">
         <v>0</v>
@@ -2380,58 +2394,58 @@
         <v>7730009</v>
       </c>
       <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" t="s">
         <v>58</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>59</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>60</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>61</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>62</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" t="s">
         <v>63</v>
       </c>
-      <c r="H5" t="s">
+      <c r="N5" t="s">
         <v>64</v>
       </c>
-      <c r="I5" t="s">
+      <c r="P5" t="s">
         <v>65</v>
       </c>
-      <c r="J5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="R5" t="s">
         <v>66</v>
       </c>
-      <c r="N5" t="s">
+      <c r="S5" t="s">
         <v>67</v>
       </c>
-      <c r="P5" t="s">
+      <c r="T5" t="s">
+        <v>66</v>
+      </c>
+      <c r="U5" t="s">
         <v>68</v>
       </c>
-      <c r="R5" t="s">
+      <c r="V5" t="s">
         <v>69</v>
-      </c>
-      <c r="S5" t="s">
-        <v>70</v>
-      </c>
-      <c r="T5" t="s">
-        <v>69</v>
-      </c>
-      <c r="U5" t="s">
-        <v>71</v>
-      </c>
-      <c r="V5" t="s">
-        <v>72</v>
       </c>
       <c r="W5">
         <v>0</v>
@@ -2442,55 +2456,55 @@
         <v>10090206</v>
       </c>
       <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" t="s">
         <v>73</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" t="s">
         <v>74</v>
       </c>
-      <c r="E6" t="s">
+      <c r="I6" t="s">
         <v>75</v>
       </c>
-      <c r="F6" t="s">
+      <c r="J6" t="s">
         <v>76</v>
       </c>
-      <c r="G6" t="s">
-        <v>76</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="K6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" t="s">
         <v>77</v>
       </c>
-      <c r="I6" t="s">
+      <c r="P6" t="s">
         <v>78</v>
       </c>
-      <c r="J6" t="s">
+      <c r="R6" t="s">
         <v>79</v>
       </c>
-      <c r="K6" t="s">
-        <v>77</v>
-      </c>
-      <c r="L6" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="S6" t="s">
         <v>80</v>
       </c>
-      <c r="P6" t="s">
+      <c r="T6" t="s">
+        <v>79</v>
+      </c>
+      <c r="U6" t="s">
         <v>81</v>
       </c>
-      <c r="R6" t="s">
+      <c r="V6" t="s">
         <v>82</v>
-      </c>
-      <c r="S6" t="s">
-        <v>83</v>
-      </c>
-      <c r="T6" t="s">
-        <v>82</v>
-      </c>
-      <c r="U6" t="s">
-        <v>84</v>
-      </c>
-      <c r="V6" t="s">
-        <v>85</v>
       </c>
       <c r="W6">
         <v>0</v>
@@ -2501,55 +2515,55 @@
         <v>10127735</v>
       </c>
       <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" t="s">
         <v>86</v>
       </c>
-      <c r="C7" t="s">
+      <c r="G7" t="s">
         <v>87</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" t="s">
         <v>88</v>
       </c>
-      <c r="F7" t="s">
+      <c r="J7" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" t="s">
         <v>89</v>
       </c>
-      <c r="G7" t="s">
+      <c r="P7" t="s">
         <v>90</v>
       </c>
-      <c r="H7" t="s">
-        <v>77</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="R7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S7" t="s">
+        <v>27</v>
+      </c>
+      <c r="T7" t="s">
         <v>91</v>
       </c>
-      <c r="J7" t="s">
-        <v>79</v>
-      </c>
-      <c r="K7" t="s">
-        <v>77</v>
-      </c>
-      <c r="L7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="U7" t="s">
         <v>92</v>
       </c>
-      <c r="P7" t="s">
+      <c r="V7" t="s">
         <v>93</v>
-      </c>
-      <c r="R7" t="s">
-        <v>28</v>
-      </c>
-      <c r="S7" t="s">
-        <v>28</v>
-      </c>
-      <c r="T7" t="s">
-        <v>94</v>
-      </c>
-      <c r="U7" t="s">
-        <v>95</v>
-      </c>
-      <c r="V7" t="s">
-        <v>96</v>
       </c>
       <c r="W7">
         <v>0</v>
@@ -2560,55 +2574,55 @@
         <v>12345878</v>
       </c>
       <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" t="s">
         <v>97</v>
       </c>
-      <c r="C8" t="s">
+      <c r="G8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" t="s">
         <v>98</v>
       </c>
-      <c r="D8" t="s">
+      <c r="I8" t="s">
         <v>99</v>
       </c>
-      <c r="E8" t="s">
+      <c r="J8" t="s">
         <v>100</v>
       </c>
-      <c r="F8" t="s">
+      <c r="L8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" t="s">
         <v>101</v>
       </c>
-      <c r="G8" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="P8" t="s">
         <v>102</v>
       </c>
-      <c r="I8" t="s">
+      <c r="R8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T8" t="s">
+        <v>99</v>
+      </c>
+      <c r="U8" t="s">
         <v>103</v>
       </c>
-      <c r="J8" t="s">
+      <c r="V8" t="s">
         <v>104</v>
-      </c>
-      <c r="L8" t="s">
-        <v>37</v>
-      </c>
-      <c r="M8" t="s">
-        <v>105</v>
-      </c>
-      <c r="P8" t="s">
-        <v>106</v>
-      </c>
-      <c r="R8" t="s">
-        <v>28</v>
-      </c>
-      <c r="S8" t="s">
-        <v>28</v>
-      </c>
-      <c r="T8" t="s">
-        <v>103</v>
-      </c>
-      <c r="U8" t="s">
-        <v>107</v>
-      </c>
-      <c r="V8" t="s">
-        <v>108</v>
       </c>
       <c r="W8">
         <v>0</v>
@@ -2619,64 +2633,64 @@
         <v>27533024</v>
       </c>
       <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" t="s">
+        <v>569</v>
+      </c>
+      <c r="E9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" t="s">
         <v>109</v>
       </c>
-      <c r="C9" t="s">
+      <c r="J9" t="s">
+        <v>100</v>
+      </c>
+      <c r="K9" t="s">
         <v>110</v>
       </c>
-      <c r="E9" t="s">
+      <c r="L9" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9" t="s">
         <v>111</v>
       </c>
-      <c r="F9" t="s">
+      <c r="N9" t="s">
         <v>112</v>
       </c>
-      <c r="G9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="O9" t="s">
         <v>113</v>
       </c>
-      <c r="I9" t="s">
+      <c r="P9" t="s">
         <v>114</v>
       </c>
-      <c r="J9" t="s">
-        <v>104</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="Q9" t="s">
         <v>115</v>
       </c>
-      <c r="L9" t="s">
-        <v>37</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="R9" t="s">
+        <v>27</v>
+      </c>
+      <c r="S9" t="s">
+        <v>27</v>
+      </c>
+      <c r="T9" t="s">
         <v>116</v>
       </c>
-      <c r="N9" t="s">
+      <c r="U9" t="s">
         <v>117</v>
       </c>
-      <c r="O9" t="s">
+      <c r="V9" t="s">
         <v>118</v>
-      </c>
-      <c r="P9" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>120</v>
-      </c>
-      <c r="R9" t="s">
-        <v>28</v>
-      </c>
-      <c r="S9" t="s">
-        <v>28</v>
-      </c>
-      <c r="T9" t="s">
-        <v>121</v>
-      </c>
-      <c r="U9" t="s">
-        <v>122</v>
-      </c>
-      <c r="V9" t="s">
-        <v>123</v>
       </c>
       <c r="W9">
         <v>0</v>
@@ -2687,64 +2701,64 @@
         <v>27533048</v>
       </c>
       <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
+        <v>570</v>
+      </c>
+      <c r="E10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10" t="s">
+        <v>108</v>
+      </c>
+      <c r="I10" t="s">
+        <v>121</v>
+      </c>
+      <c r="J10" t="s">
+        <v>100</v>
+      </c>
+      <c r="K10" t="s">
+        <v>110</v>
+      </c>
+      <c r="L10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" t="s">
+        <v>122</v>
+      </c>
+      <c r="N10" t="s">
+        <v>123</v>
+      </c>
+      <c r="O10" t="s">
+        <v>113</v>
+      </c>
+      <c r="P10" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>115</v>
+      </c>
+      <c r="R10" t="s">
+        <v>66</v>
+      </c>
+      <c r="S10" t="s">
+        <v>67</v>
+      </c>
+      <c r="T10" t="s">
+        <v>66</v>
+      </c>
+      <c r="U10" t="s">
         <v>124</v>
       </c>
-      <c r="C10" t="s">
-        <v>110</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="V10" t="s">
         <v>125</v>
-      </c>
-      <c r="F10" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" t="s">
-        <v>112</v>
-      </c>
-      <c r="H10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I10" t="s">
-        <v>126</v>
-      </c>
-      <c r="J10" t="s">
-        <v>104</v>
-      </c>
-      <c r="K10" t="s">
-        <v>115</v>
-      </c>
-      <c r="L10" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" t="s">
-        <v>127</v>
-      </c>
-      <c r="N10" t="s">
-        <v>128</v>
-      </c>
-      <c r="O10" t="s">
-        <v>118</v>
-      </c>
-      <c r="P10" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>120</v>
-      </c>
-      <c r="R10" t="s">
-        <v>69</v>
-      </c>
-      <c r="S10" t="s">
-        <v>70</v>
-      </c>
-      <c r="T10" t="s">
-        <v>69</v>
-      </c>
-      <c r="U10" t="s">
-        <v>129</v>
-      </c>
-      <c r="V10" t="s">
-        <v>130</v>
       </c>
       <c r="W10">
         <v>0</v>
@@ -2755,28 +2769,28 @@
         <v>30053014</v>
       </c>
       <c r="B11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" t="s">
+        <v>129</v>
+      </c>
+      <c r="L11" t="s">
+        <v>26</v>
+      </c>
+      <c r="U11" t="s">
+        <v>130</v>
+      </c>
+      <c r="V11" t="s">
         <v>131</v>
-      </c>
-      <c r="C11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F11" t="s">
-        <v>134</v>
-      </c>
-      <c r="G11" t="s">
-        <v>134</v>
-      </c>
-      <c r="L11" t="s">
-        <v>27</v>
-      </c>
-      <c r="U11" t="s">
-        <v>135</v>
-      </c>
-      <c r="V11" t="s">
-        <v>136</v>
       </c>
       <c r="W11">
         <v>0</v>
@@ -2787,61 +2801,61 @@
         <v>40608754</v>
       </c>
       <c r="B12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="D12" t="s">
+        <v>133</v>
+      </c>
+      <c r="E12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G12" t="s">
+        <v>136</v>
+      </c>
+      <c r="H12" t="s">
         <v>137</v>
       </c>
-      <c r="C12" t="s">
+      <c r="I12" t="s">
         <v>138</v>
       </c>
-      <c r="D12" t="s">
+      <c r="J12" t="s">
         <v>139</v>
       </c>
-      <c r="E12" t="s">
+      <c r="L12" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" t="s">
         <v>140</v>
       </c>
-      <c r="F12" t="s">
+      <c r="O12" t="s">
         <v>141</v>
       </c>
-      <c r="G12" t="s">
+      <c r="P12" t="s">
         <v>142</v>
       </c>
-      <c r="H12" t="s">
+      <c r="Q12" t="s">
         <v>143</v>
       </c>
-      <c r="I12" t="s">
+      <c r="R12" t="s">
+        <v>79</v>
+      </c>
+      <c r="S12" t="s">
         <v>144</v>
       </c>
-      <c r="J12" t="s">
+      <c r="T12" t="s">
+        <v>79</v>
+      </c>
+      <c r="U12" t="s">
         <v>145</v>
       </c>
-      <c r="L12" t="s">
-        <v>27</v>
-      </c>
-      <c r="M12" t="s">
+      <c r="V12" t="s">
         <v>146</v>
-      </c>
-      <c r="O12" t="s">
-        <v>147</v>
-      </c>
-      <c r="P12" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>149</v>
-      </c>
-      <c r="R12" t="s">
-        <v>82</v>
-      </c>
-      <c r="S12" t="s">
-        <v>150</v>
-      </c>
-      <c r="T12" t="s">
-        <v>82</v>
-      </c>
-      <c r="U12" t="s">
-        <v>151</v>
-      </c>
-      <c r="V12" t="s">
-        <v>152</v>
       </c>
       <c r="W12">
         <v>0</v>
@@ -2852,58 +2866,58 @@
         <v>758</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D13" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
+        <v>149</v>
+      </c>
+      <c r="G13" t="s">
+        <v>150</v>
+      </c>
+      <c r="H13" t="s">
+        <v>151</v>
+      </c>
+      <c r="I13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J13" t="s">
+        <v>100</v>
+      </c>
+      <c r="K13" t="s">
+        <v>153</v>
+      </c>
+      <c r="L13" t="s">
+        <v>36</v>
+      </c>
+      <c r="M13" t="s">
+        <v>148</v>
+      </c>
+      <c r="P13" t="s">
+        <v>154</v>
+      </c>
+      <c r="R13" t="s">
         <v>155</v>
       </c>
-      <c r="G13" t="s">
+      <c r="S13" t="s">
         <v>156</v>
       </c>
-      <c r="H13" t="s">
+      <c r="T13" t="s">
+        <v>42</v>
+      </c>
+      <c r="U13" t="s">
         <v>157</v>
       </c>
-      <c r="I13" t="s">
+      <c r="V13" t="s">
         <v>158</v>
-      </c>
-      <c r="J13" t="s">
-        <v>104</v>
-      </c>
-      <c r="K13" t="s">
-        <v>159</v>
-      </c>
-      <c r="L13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M13" t="s">
-        <v>154</v>
-      </c>
-      <c r="P13" t="s">
-        <v>160</v>
-      </c>
-      <c r="R13" t="s">
-        <v>161</v>
-      </c>
-      <c r="S13" t="s">
-        <v>162</v>
-      </c>
-      <c r="T13" t="s">
-        <v>43</v>
-      </c>
-      <c r="U13" t="s">
-        <v>163</v>
-      </c>
-      <c r="V13" t="s">
-        <v>164</v>
       </c>
       <c r="W13">
         <v>0</v>
@@ -2914,61 +2928,61 @@
         <v>84154071</v>
       </c>
       <c r="B14" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" t="s">
+        <v>160</v>
+      </c>
+      <c r="D14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14" t="s">
+        <v>161</v>
+      </c>
+      <c r="F14" t="s">
+        <v>571</v>
+      </c>
+      <c r="G14" t="s">
+        <v>162</v>
+      </c>
+      <c r="H14" t="s">
+        <v>163</v>
+      </c>
+      <c r="I14" t="s">
+        <v>164</v>
+      </c>
+      <c r="J14" t="s">
         <v>165</v>
       </c>
-      <c r="C14" t="s">
+      <c r="K14" t="s">
         <v>166</v>
       </c>
-      <c r="D14" t="s">
-        <v>166</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="L14" t="s">
         <v>167</v>
       </c>
-      <c r="F14" t="s">
+      <c r="M14" t="s">
         <v>168</v>
       </c>
-      <c r="G14" t="s">
+      <c r="N14" t="s">
         <v>169</v>
       </c>
-      <c r="H14" t="s">
+      <c r="P14" t="s">
         <v>170</v>
       </c>
-      <c r="I14" t="s">
+      <c r="R14" t="s">
         <v>171</v>
       </c>
-      <c r="J14" t="s">
+      <c r="S14" t="s">
         <v>172</v>
       </c>
-      <c r="K14" t="s">
+      <c r="T14" t="s">
         <v>173</v>
       </c>
-      <c r="L14" t="s">
+      <c r="U14" t="s">
         <v>174</v>
       </c>
-      <c r="M14" t="s">
+      <c r="V14" t="s">
         <v>175</v>
-      </c>
-      <c r="N14" t="s">
-        <v>176</v>
-      </c>
-      <c r="P14" t="s">
-        <v>177</v>
-      </c>
-      <c r="R14" t="s">
-        <v>178</v>
-      </c>
-      <c r="S14" t="s">
-        <v>179</v>
-      </c>
-      <c r="T14" t="s">
-        <v>180</v>
-      </c>
-      <c r="U14" t="s">
-        <v>181</v>
-      </c>
-      <c r="V14" t="s">
-        <v>182</v>
       </c>
       <c r="W14">
         <v>0</v>
@@ -2979,64 +2993,64 @@
         <v>87177756</v>
       </c>
       <c r="B15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D15" t="s">
+        <v>178</v>
+      </c>
+      <c r="E15" t="s">
+        <v>179</v>
+      </c>
+      <c r="F15" t="s">
+        <v>180</v>
+      </c>
+      <c r="G15" t="s">
+        <v>181</v>
+      </c>
+      <c r="H15" t="s">
+        <v>182</v>
+      </c>
+      <c r="I15" t="s">
         <v>183</v>
       </c>
-      <c r="C15" t="s">
+      <c r="J15" t="s">
         <v>184</v>
       </c>
-      <c r="D15" t="s">
+      <c r="K15" t="s">
         <v>185</v>
       </c>
-      <c r="E15" t="s">
+      <c r="L15" t="s">
+        <v>26</v>
+      </c>
+      <c r="M15" t="s">
         <v>186</v>
       </c>
-      <c r="F15" t="s">
+      <c r="O15" t="s">
+        <v>179</v>
+      </c>
+      <c r="P15" t="s">
         <v>187</v>
       </c>
-      <c r="G15" t="s">
+      <c r="Q15" t="s">
+        <v>143</v>
+      </c>
+      <c r="R15" t="s">
+        <v>79</v>
+      </c>
+      <c r="S15" t="s">
+        <v>144</v>
+      </c>
+      <c r="T15" t="s">
+        <v>79</v>
+      </c>
+      <c r="U15" t="s">
         <v>188</v>
       </c>
-      <c r="H15" t="s">
+      <c r="V15" t="s">
         <v>189</v>
-      </c>
-      <c r="I15" t="s">
-        <v>190</v>
-      </c>
-      <c r="J15" t="s">
-        <v>191</v>
-      </c>
-      <c r="K15" t="s">
-        <v>192</v>
-      </c>
-      <c r="L15" t="s">
-        <v>27</v>
-      </c>
-      <c r="M15" t="s">
-        <v>193</v>
-      </c>
-      <c r="O15" t="s">
-        <v>186</v>
-      </c>
-      <c r="P15" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>149</v>
-      </c>
-      <c r="R15" t="s">
-        <v>82</v>
-      </c>
-      <c r="S15" t="s">
-        <v>150</v>
-      </c>
-      <c r="T15" t="s">
-        <v>82</v>
-      </c>
-      <c r="U15" t="s">
-        <v>195</v>
-      </c>
-      <c r="V15" t="s">
-        <v>196</v>
       </c>
       <c r="W15">
         <v>0</v>
@@ -3047,55 +3061,55 @@
         <v>1373</v>
       </c>
       <c r="B16" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C16" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="E16">
         <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="G16" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="H16" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="I16" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="J16" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K16" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="L16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M16" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="P16" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="R16" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="S16" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="T16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U16" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="V16" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="W16">
         <v>0</v>
@@ -3106,55 +3120,55 @@
         <v>2929</v>
       </c>
       <c r="B17" t="s">
+        <v>198</v>
+      </c>
+      <c r="C17" t="s">
+        <v>199</v>
+      </c>
+      <c r="E17" t="s">
+        <v>200</v>
+      </c>
+      <c r="F17" t="s">
+        <v>201</v>
+      </c>
+      <c r="G17" t="s">
+        <v>202</v>
+      </c>
+      <c r="H17" t="s">
+        <v>203</v>
+      </c>
+      <c r="I17" t="s">
+        <v>204</v>
+      </c>
+      <c r="J17" t="s">
         <v>205</v>
       </c>
-      <c r="C17" t="s">
+      <c r="K17" t="s">
         <v>206</v>
       </c>
-      <c r="E17" t="s">
+      <c r="L17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" t="s">
         <v>207</v>
       </c>
-      <c r="F17" t="s">
+      <c r="P17" t="s">
         <v>208</v>
       </c>
-      <c r="G17" t="s">
+      <c r="R17" t="s">
+        <v>27</v>
+      </c>
+      <c r="S17" t="s">
+        <v>27</v>
+      </c>
+      <c r="T17" t="s">
+        <v>173</v>
+      </c>
+      <c r="U17" t="s">
         <v>209</v>
       </c>
-      <c r="H17" t="s">
+      <c r="V17" t="s">
         <v>210</v>
-      </c>
-      <c r="I17" t="s">
-        <v>211</v>
-      </c>
-      <c r="J17" t="s">
-        <v>212</v>
-      </c>
-      <c r="K17" t="s">
-        <v>213</v>
-      </c>
-      <c r="L17" t="s">
-        <v>37</v>
-      </c>
-      <c r="M17" t="s">
-        <v>214</v>
-      </c>
-      <c r="P17" t="s">
-        <v>215</v>
-      </c>
-      <c r="R17" t="s">
-        <v>28</v>
-      </c>
-      <c r="S17" t="s">
-        <v>28</v>
-      </c>
-      <c r="T17" t="s">
-        <v>180</v>
-      </c>
-      <c r="U17" t="s">
-        <v>216</v>
-      </c>
-      <c r="V17" t="s">
-        <v>217</v>
       </c>
       <c r="W17">
         <v>0</v>
@@ -3165,49 +3179,49 @@
         <v>3100</v>
       </c>
       <c r="B18" t="s">
+        <v>211</v>
+      </c>
+      <c r="C18" t="s">
+        <v>212</v>
+      </c>
+      <c r="E18" t="s">
+        <v>213</v>
+      </c>
+      <c r="F18" t="s">
+        <v>214</v>
+      </c>
+      <c r="G18" t="s">
+        <v>215</v>
+      </c>
+      <c r="H18" t="s">
+        <v>216</v>
+      </c>
+      <c r="I18" t="s">
+        <v>217</v>
+      </c>
+      <c r="L18" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" t="s">
         <v>218</v>
       </c>
-      <c r="C18" t="s">
+      <c r="P18" t="s">
         <v>219</v>
       </c>
-      <c r="E18" t="s">
+      <c r="R18" t="s">
         <v>220</v>
       </c>
-      <c r="F18" t="s">
+      <c r="S18" t="s">
         <v>221</v>
       </c>
-      <c r="G18" t="s">
+      <c r="T18" t="s">
         <v>222</v>
       </c>
-      <c r="H18" t="s">
+      <c r="U18" t="s">
         <v>223</v>
       </c>
-      <c r="I18" t="s">
+      <c r="V18" t="s">
         <v>224</v>
-      </c>
-      <c r="L18" t="s">
-        <v>27</v>
-      </c>
-      <c r="M18" t="s">
-        <v>225</v>
-      </c>
-      <c r="P18" t="s">
-        <v>226</v>
-      </c>
-      <c r="R18" t="s">
-        <v>227</v>
-      </c>
-      <c r="S18" t="s">
-        <v>228</v>
-      </c>
-      <c r="T18" t="s">
-        <v>229</v>
-      </c>
-      <c r="U18" t="s">
-        <v>230</v>
-      </c>
-      <c r="V18" t="s">
-        <v>231</v>
       </c>
       <c r="W18">
         <v>0</v>
@@ -3218,46 +3232,46 @@
         <v>790310044</v>
       </c>
       <c r="B19" t="s">
+        <v>225</v>
+      </c>
+      <c r="C19" t="s">
+        <v>226</v>
+      </c>
+      <c r="D19" t="s">
+        <v>227</v>
+      </c>
+      <c r="E19" t="s">
+        <v>228</v>
+      </c>
+      <c r="F19" t="s">
+        <v>229</v>
+      </c>
+      <c r="G19" t="s">
+        <v>230</v>
+      </c>
+      <c r="H19" t="s">
+        <v>231</v>
+      </c>
+      <c r="I19" t="s">
         <v>232</v>
       </c>
-      <c r="C19" t="s">
+      <c r="L19" t="s">
         <v>233</v>
       </c>
-      <c r="D19" t="s">
+      <c r="R19" t="s">
+        <v>66</v>
+      </c>
+      <c r="S19" t="s">
         <v>234</v>
       </c>
-      <c r="E19" t="s">
+      <c r="T19" t="s">
+        <v>66</v>
+      </c>
+      <c r="U19" t="s">
         <v>235</v>
       </c>
-      <c r="F19" t="s">
+      <c r="V19" t="s">
         <v>236</v>
-      </c>
-      <c r="G19" t="s">
-        <v>237</v>
-      </c>
-      <c r="H19" t="s">
-        <v>238</v>
-      </c>
-      <c r="I19" t="s">
-        <v>239</v>
-      </c>
-      <c r="L19" t="s">
-        <v>240</v>
-      </c>
-      <c r="R19" t="s">
-        <v>69</v>
-      </c>
-      <c r="S19" t="s">
-        <v>241</v>
-      </c>
-      <c r="T19" t="s">
-        <v>69</v>
-      </c>
-      <c r="U19" t="s">
-        <v>242</v>
-      </c>
-      <c r="V19" t="s">
-        <v>243</v>
       </c>
       <c r="W19">
         <v>0</v>
@@ -3268,43 +3282,43 @@
         <v>886100252</v>
       </c>
       <c r="B20" t="s">
-        <v>244</v>
-      </c>
-      <c r="C20" t="s">
-        <v>143</v>
+        <v>237</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>572</v>
       </c>
       <c r="E20" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="F20" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="G20" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="H20" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="I20" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="L20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R20" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="S20" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="T20" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="U20" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="V20" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="W20">
         <v>0</v>
@@ -3315,61 +3329,61 @@
         <v>104</v>
       </c>
       <c r="B21" t="s">
+        <v>242</v>
+      </c>
+      <c r="C21" t="s">
+        <v>243</v>
+      </c>
+      <c r="D21" t="s">
+        <v>244</v>
+      </c>
+      <c r="E21" t="s">
+        <v>245</v>
+      </c>
+      <c r="F21" t="s">
+        <v>246</v>
+      </c>
+      <c r="G21" t="s">
+        <v>247</v>
+      </c>
+      <c r="H21" t="s">
+        <v>248</v>
+      </c>
+      <c r="I21" t="s">
         <v>249</v>
       </c>
-      <c r="C21" t="s">
+      <c r="J21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L21" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" t="s">
         <v>250</v>
       </c>
-      <c r="D21" t="s">
+      <c r="O21" t="s">
         <v>251</v>
       </c>
-      <c r="E21" t="s">
+      <c r="P21" t="s">
         <v>252</v>
       </c>
-      <c r="F21" t="s">
+      <c r="Q21" t="s">
         <v>253</v>
       </c>
-      <c r="G21" t="s">
+      <c r="R21" t="s">
+        <v>66</v>
+      </c>
+      <c r="S21" t="s">
+        <v>67</v>
+      </c>
+      <c r="T21" t="s">
+        <v>66</v>
+      </c>
+      <c r="U21" t="s">
         <v>254</v>
       </c>
-      <c r="H21" t="s">
+      <c r="V21" t="s">
         <v>255</v>
-      </c>
-      <c r="I21" t="s">
-        <v>256</v>
-      </c>
-      <c r="J21" t="s">
-        <v>27</v>
-      </c>
-      <c r="L21" t="s">
-        <v>27</v>
-      </c>
-      <c r="M21" t="s">
-        <v>257</v>
-      </c>
-      <c r="O21" t="s">
-        <v>258</v>
-      </c>
-      <c r="P21" t="s">
-        <v>259</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>260</v>
-      </c>
-      <c r="R21" t="s">
-        <v>69</v>
-      </c>
-      <c r="S21" t="s">
-        <v>70</v>
-      </c>
-      <c r="T21" t="s">
-        <v>69</v>
-      </c>
-      <c r="U21" t="s">
-        <v>261</v>
-      </c>
-      <c r="V21" t="s">
-        <v>262</v>
       </c>
       <c r="W21">
         <v>0</v>
@@ -3380,40 +3394,40 @@
         <v>11021096</v>
       </c>
       <c r="B22" t="s">
+        <v>256</v>
+      </c>
+      <c r="C22" t="s">
+        <v>257</v>
+      </c>
+      <c r="E22" t="s">
+        <v>258</v>
+      </c>
+      <c r="F22" t="s">
+        <v>259</v>
+      </c>
+      <c r="G22" t="s">
+        <v>260</v>
+      </c>
+      <c r="I22" t="s">
+        <v>261</v>
+      </c>
+      <c r="L22" t="s">
+        <v>26</v>
+      </c>
+      <c r="R22" t="s">
+        <v>27</v>
+      </c>
+      <c r="S22" t="s">
+        <v>27</v>
+      </c>
+      <c r="T22" t="s">
+        <v>262</v>
+      </c>
+      <c r="U22" t="s">
         <v>263</v>
       </c>
-      <c r="C22" t="s">
+      <c r="V22" t="s">
         <v>264</v>
-      </c>
-      <c r="E22" t="s">
-        <v>265</v>
-      </c>
-      <c r="F22" t="s">
-        <v>266</v>
-      </c>
-      <c r="G22" t="s">
-        <v>267</v>
-      </c>
-      <c r="I22" t="s">
-        <v>268</v>
-      </c>
-      <c r="L22" t="s">
-        <v>27</v>
-      </c>
-      <c r="R22" t="s">
-        <v>28</v>
-      </c>
-      <c r="S22" t="s">
-        <v>28</v>
-      </c>
-      <c r="T22" t="s">
-        <v>269</v>
-      </c>
-      <c r="U22" t="s">
-        <v>270</v>
-      </c>
-      <c r="V22" t="s">
-        <v>271</v>
       </c>
       <c r="W22">
         <v>0</v>
@@ -3424,28 +3438,28 @@
         <v>1109205</v>
       </c>
       <c r="B23" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C23" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E23" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="F23" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="G23" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="L23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U23" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="V23" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="W23">
         <v>0</v>
@@ -3456,40 +3470,40 @@
         <v>11201096</v>
       </c>
       <c r="B24" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="C24" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="E24" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F24" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="G24" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="I24" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="L24" t="s">
+        <v>26</v>
+      </c>
+      <c r="R24" t="s">
         <v>27</v>
       </c>
-      <c r="R24" t="s">
-        <v>28</v>
-      </c>
       <c r="S24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T24" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="U24" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="V24" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="W24">
         <v>0</v>
@@ -3500,40 +3514,40 @@
         <v>11251085</v>
       </c>
       <c r="B25" t="s">
+        <v>275</v>
+      </c>
+      <c r="C25" t="s">
+        <v>276</v>
+      </c>
+      <c r="E25" t="s">
+        <v>277</v>
+      </c>
+      <c r="F25" t="s">
+        <v>278</v>
+      </c>
+      <c r="G25" t="s">
+        <v>279</v>
+      </c>
+      <c r="I25" t="s">
+        <v>280</v>
+      </c>
+      <c r="L25" t="s">
+        <v>26</v>
+      </c>
+      <c r="R25" t="s">
+        <v>27</v>
+      </c>
+      <c r="S25" t="s">
+        <v>27</v>
+      </c>
+      <c r="T25" t="s">
+        <v>262</v>
+      </c>
+      <c r="U25" t="s">
+        <v>281</v>
+      </c>
+      <c r="V25" t="s">
         <v>282</v>
-      </c>
-      <c r="C25" t="s">
-        <v>283</v>
-      </c>
-      <c r="E25" t="s">
-        <v>284</v>
-      </c>
-      <c r="F25" t="s">
-        <v>285</v>
-      </c>
-      <c r="G25" t="s">
-        <v>286</v>
-      </c>
-      <c r="I25" t="s">
-        <v>287</v>
-      </c>
-      <c r="L25" t="s">
-        <v>27</v>
-      </c>
-      <c r="R25" t="s">
-        <v>28</v>
-      </c>
-      <c r="S25" t="s">
-        <v>28</v>
-      </c>
-      <c r="T25" t="s">
-        <v>269</v>
-      </c>
-      <c r="U25" t="s">
-        <v>288</v>
-      </c>
-      <c r="V25" t="s">
-        <v>289</v>
       </c>
       <c r="W25">
         <v>0</v>
@@ -3544,43 +3558,43 @@
         <v>11281070</v>
       </c>
       <c r="B26" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="C26" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E26" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="F26" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="G26" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="H26" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="I26" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="L26" t="s">
+        <v>26</v>
+      </c>
+      <c r="R26" t="s">
         <v>27</v>
       </c>
-      <c r="R26" t="s">
-        <v>28</v>
-      </c>
       <c r="S26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T26" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="U26" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="V26" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="W26">
         <v>0</v>
@@ -3591,43 +3605,43 @@
         <v>11281076</v>
       </c>
       <c r="B27" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="C27" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="E27" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F27" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="G27" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="H27" t="s">
+        <v>286</v>
+      </c>
+      <c r="I27" t="s">
+        <v>287</v>
+      </c>
+      <c r="L27" t="s">
+        <v>26</v>
+      </c>
+      <c r="R27" t="s">
+        <v>27</v>
+      </c>
+      <c r="S27" t="s">
+        <v>27</v>
+      </c>
+      <c r="T27" t="s">
+        <v>262</v>
+      </c>
+      <c r="U27" t="s">
+        <v>292</v>
+      </c>
+      <c r="V27" t="s">
         <v>293</v>
-      </c>
-      <c r="I27" t="s">
-        <v>294</v>
-      </c>
-      <c r="L27" t="s">
-        <v>27</v>
-      </c>
-      <c r="R27" t="s">
-        <v>28</v>
-      </c>
-      <c r="S27" t="s">
-        <v>28</v>
-      </c>
-      <c r="T27" t="s">
-        <v>269</v>
-      </c>
-      <c r="U27" t="s">
-        <v>299</v>
-      </c>
-      <c r="V27" t="s">
-        <v>300</v>
       </c>
       <c r="W27">
         <v>0</v>
@@ -3638,61 +3652,61 @@
         <v>11501</v>
       </c>
       <c r="B28" t="s">
+        <v>294</v>
+      </c>
+      <c r="C28" t="s">
+        <v>295</v>
+      </c>
+      <c r="D28" t="s">
+        <v>296</v>
+      </c>
+      <c r="E28" t="s">
+        <v>297</v>
+      </c>
+      <c r="F28" t="s">
+        <v>298</v>
+      </c>
+      <c r="G28" t="s">
+        <v>298</v>
+      </c>
+      <c r="H28" t="s">
+        <v>206</v>
+      </c>
+      <c r="I28" t="s">
+        <v>299</v>
+      </c>
+      <c r="J28" t="s">
+        <v>100</v>
+      </c>
+      <c r="K28" t="s">
+        <v>206</v>
+      </c>
+      <c r="L28" t="s">
+        <v>300</v>
+      </c>
+      <c r="M28" t="s">
         <v>301</v>
       </c>
-      <c r="C28" t="s">
+      <c r="P28" t="s">
         <v>302</v>
       </c>
-      <c r="D28" t="s">
+      <c r="Q28" t="s">
+        <v>253</v>
+      </c>
+      <c r="R28" t="s">
+        <v>27</v>
+      </c>
+      <c r="S28" t="s">
+        <v>27</v>
+      </c>
+      <c r="T28" t="s">
+        <v>173</v>
+      </c>
+      <c r="U28" t="s">
         <v>303</v>
       </c>
-      <c r="E28" t="s">
+      <c r="V28" t="s">
         <v>304</v>
-      </c>
-      <c r="F28" t="s">
-        <v>305</v>
-      </c>
-      <c r="G28" t="s">
-        <v>305</v>
-      </c>
-      <c r="H28" t="s">
-        <v>213</v>
-      </c>
-      <c r="I28" t="s">
-        <v>306</v>
-      </c>
-      <c r="J28" t="s">
-        <v>104</v>
-      </c>
-      <c r="K28" t="s">
-        <v>213</v>
-      </c>
-      <c r="L28" t="s">
-        <v>307</v>
-      </c>
-      <c r="M28" t="s">
-        <v>308</v>
-      </c>
-      <c r="P28" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>260</v>
-      </c>
-      <c r="R28" t="s">
-        <v>28</v>
-      </c>
-      <c r="S28" t="s">
-        <v>28</v>
-      </c>
-      <c r="T28" t="s">
-        <v>180</v>
-      </c>
-      <c r="U28" t="s">
-        <v>310</v>
-      </c>
-      <c r="V28" t="s">
-        <v>311</v>
       </c>
       <c r="W28">
         <v>0</v>
@@ -3703,52 +3717,52 @@
         <v>11693</v>
       </c>
       <c r="B29" t="s">
+        <v>305</v>
+      </c>
+      <c r="C29" t="s">
+        <v>306</v>
+      </c>
+      <c r="D29" t="s">
+        <v>307</v>
+      </c>
+      <c r="E29" t="s">
+        <v>308</v>
+      </c>
+      <c r="F29" t="s">
+        <v>309</v>
+      </c>
+      <c r="G29" t="s">
+        <v>310</v>
+      </c>
+      <c r="H29" t="s">
+        <v>311</v>
+      </c>
+      <c r="I29" t="s">
         <v>312</v>
       </c>
-      <c r="C29" t="s">
+      <c r="L29" t="s">
+        <v>26</v>
+      </c>
+      <c r="O29" t="s">
         <v>313</v>
       </c>
-      <c r="D29" t="s">
+      <c r="Q29" t="s">
+        <v>143</v>
+      </c>
+      <c r="R29" t="s">
+        <v>66</v>
+      </c>
+      <c r="S29" t="s">
+        <v>67</v>
+      </c>
+      <c r="T29" t="s">
+        <v>66</v>
+      </c>
+      <c r="U29" t="s">
         <v>314</v>
       </c>
-      <c r="E29" t="s">
+      <c r="V29" t="s">
         <v>315</v>
-      </c>
-      <c r="F29" t="s">
-        <v>316</v>
-      </c>
-      <c r="G29" t="s">
-        <v>317</v>
-      </c>
-      <c r="H29" t="s">
-        <v>318</v>
-      </c>
-      <c r="I29" t="s">
-        <v>319</v>
-      </c>
-      <c r="L29" t="s">
-        <v>27</v>
-      </c>
-      <c r="O29" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>149</v>
-      </c>
-      <c r="R29" t="s">
-        <v>69</v>
-      </c>
-      <c r="S29" t="s">
-        <v>70</v>
-      </c>
-      <c r="T29" t="s">
-        <v>69</v>
-      </c>
-      <c r="U29" t="s">
-        <v>321</v>
-      </c>
-      <c r="V29" t="s">
-        <v>322</v>
       </c>
       <c r="W29">
         <v>0</v>
@@ -3759,61 +3773,61 @@
         <v>11815</v>
       </c>
       <c r="B30" t="s">
+        <v>316</v>
+      </c>
+      <c r="C30" t="s">
+        <v>317</v>
+      </c>
+      <c r="D30" t="s">
+        <v>318</v>
+      </c>
+      <c r="E30" t="s">
+        <v>319</v>
+      </c>
+      <c r="F30" t="s">
+        <v>320</v>
+      </c>
+      <c r="G30" t="s">
+        <v>321</v>
+      </c>
+      <c r="H30" t="s">
+        <v>322</v>
+      </c>
+      <c r="I30" t="s">
+        <v>312</v>
+      </c>
+      <c r="L30" t="s">
+        <v>26</v>
+      </c>
+      <c r="M30" t="s">
         <v>323</v>
       </c>
-      <c r="C30" t="s">
+      <c r="N30" t="s">
         <v>324</v>
       </c>
-      <c r="D30" t="s">
+      <c r="O30" t="s">
         <v>325</v>
       </c>
-      <c r="E30" t="s">
+      <c r="P30" t="s">
         <v>326</v>
       </c>
-      <c r="F30" t="s">
+      <c r="Q30" t="s">
+        <v>143</v>
+      </c>
+      <c r="R30" t="s">
+        <v>66</v>
+      </c>
+      <c r="S30" t="s">
+        <v>67</v>
+      </c>
+      <c r="T30" t="s">
+        <v>66</v>
+      </c>
+      <c r="U30" t="s">
         <v>327</v>
       </c>
-      <c r="G30" t="s">
+      <c r="V30" t="s">
         <v>328</v>
-      </c>
-      <c r="H30" t="s">
-        <v>329</v>
-      </c>
-      <c r="I30" t="s">
-        <v>319</v>
-      </c>
-      <c r="L30" t="s">
-        <v>27</v>
-      </c>
-      <c r="M30" t="s">
-        <v>330</v>
-      </c>
-      <c r="N30" t="s">
-        <v>331</v>
-      </c>
-      <c r="O30" t="s">
-        <v>332</v>
-      </c>
-      <c r="P30" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>149</v>
-      </c>
-      <c r="R30" t="s">
-        <v>69</v>
-      </c>
-      <c r="S30" t="s">
-        <v>70</v>
-      </c>
-      <c r="T30" t="s">
-        <v>69</v>
-      </c>
-      <c r="U30" t="s">
-        <v>334</v>
-      </c>
-      <c r="V30" t="s">
-        <v>335</v>
       </c>
       <c r="W30">
         <v>0</v>
@@ -3824,55 +3838,55 @@
         <v>19170</v>
       </c>
       <c r="B31" t="s">
+        <v>329</v>
+      </c>
+      <c r="C31" t="s">
+        <v>330</v>
+      </c>
+      <c r="E31" t="s">
+        <v>331</v>
+      </c>
+      <c r="F31" t="s">
+        <v>332</v>
+      </c>
+      <c r="G31" t="s">
+        <v>332</v>
+      </c>
+      <c r="H31" t="s">
+        <v>151</v>
+      </c>
+      <c r="I31" t="s">
+        <v>333</v>
+      </c>
+      <c r="J31" t="s">
+        <v>100</v>
+      </c>
+      <c r="K31" t="s">
+        <v>153</v>
+      </c>
+      <c r="L31" t="s">
+        <v>36</v>
+      </c>
+      <c r="M31" t="s">
+        <v>330</v>
+      </c>
+      <c r="P31" t="s">
+        <v>334</v>
+      </c>
+      <c r="R31" t="s">
+        <v>335</v>
+      </c>
+      <c r="S31" t="s">
         <v>336</v>
       </c>
-      <c r="C31" t="s">
+      <c r="T31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U31" t="s">
         <v>337</v>
       </c>
-      <c r="E31" t="s">
+      <c r="V31" t="s">
         <v>338</v>
-      </c>
-      <c r="F31" t="s">
-        <v>339</v>
-      </c>
-      <c r="G31" t="s">
-        <v>339</v>
-      </c>
-      <c r="H31" t="s">
-        <v>157</v>
-      </c>
-      <c r="I31" t="s">
-        <v>340</v>
-      </c>
-      <c r="J31" t="s">
-        <v>104</v>
-      </c>
-      <c r="K31" t="s">
-        <v>159</v>
-      </c>
-      <c r="L31" t="s">
-        <v>37</v>
-      </c>
-      <c r="M31" t="s">
-        <v>337</v>
-      </c>
-      <c r="P31" t="s">
-        <v>341</v>
-      </c>
-      <c r="R31" t="s">
-        <v>342</v>
-      </c>
-      <c r="S31" t="s">
-        <v>343</v>
-      </c>
-      <c r="T31" t="s">
-        <v>43</v>
-      </c>
-      <c r="U31" t="s">
-        <v>344</v>
-      </c>
-      <c r="V31" t="s">
-        <v>345</v>
       </c>
       <c r="W31">
         <v>0</v>
@@ -3883,25 +3897,25 @@
         <v>24136</v>
       </c>
       <c r="B32" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="C32" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="F32" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="G32" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="L32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U32" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="V32" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="W32">
         <v>0</v>
@@ -3912,58 +3926,58 @@
         <v>25157</v>
       </c>
       <c r="B33" t="s">
+        <v>344</v>
+      </c>
+      <c r="C33" t="s">
+        <v>345</v>
+      </c>
+      <c r="E33" t="s">
+        <v>346</v>
+      </c>
+      <c r="F33" t="s">
+        <v>347</v>
+      </c>
+      <c r="G33" t="s">
+        <v>348</v>
+      </c>
+      <c r="H33" t="s">
+        <v>349</v>
+      </c>
+      <c r="I33" t="s">
+        <v>350</v>
+      </c>
+      <c r="L33" t="s">
+        <v>233</v>
+      </c>
+      <c r="M33" t="s">
         <v>351</v>
       </c>
-      <c r="C33" t="s">
+      <c r="N33" t="s">
         <v>352</v>
       </c>
-      <c r="E33" t="s">
+      <c r="O33" t="s">
         <v>353</v>
       </c>
-      <c r="F33" t="s">
+      <c r="P33" t="s">
         <v>354</v>
       </c>
-      <c r="G33" t="s">
+      <c r="Q33" t="s">
+        <v>253</v>
+      </c>
+      <c r="R33" t="s">
         <v>355</v>
       </c>
-      <c r="H33" t="s">
+      <c r="S33" t="s">
         <v>356</v>
       </c>
-      <c r="I33" t="s">
+      <c r="T33" t="s">
         <v>357</v>
       </c>
-      <c r="L33" t="s">
-        <v>240</v>
-      </c>
-      <c r="M33" t="s">
+      <c r="U33" t="s">
         <v>358</v>
       </c>
-      <c r="N33" t="s">
+      <c r="V33" t="s">
         <v>359</v>
-      </c>
-      <c r="O33" t="s">
-        <v>360</v>
-      </c>
-      <c r="P33" t="s">
-        <v>361</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>260</v>
-      </c>
-      <c r="R33" t="s">
-        <v>362</v>
-      </c>
-      <c r="S33" t="s">
-        <v>363</v>
-      </c>
-      <c r="T33" t="s">
-        <v>364</v>
-      </c>
-      <c r="U33" t="s">
-        <v>365</v>
-      </c>
-      <c r="V33" t="s">
-        <v>366</v>
       </c>
       <c r="W33">
         <v>0</v>
@@ -3974,61 +3988,61 @@
         <v>25751</v>
       </c>
       <c r="B34" t="s">
+        <v>360</v>
+      </c>
+      <c r="C34" t="s">
+        <v>361</v>
+      </c>
+      <c r="D34" t="s">
+        <v>362</v>
+      </c>
+      <c r="E34" t="s">
+        <v>363</v>
+      </c>
+      <c r="F34" t="s">
+        <v>364</v>
+      </c>
+      <c r="G34" t="s">
+        <v>215</v>
+      </c>
+      <c r="H34" t="s">
+        <v>365</v>
+      </c>
+      <c r="I34" t="s">
+        <v>366</v>
+      </c>
+      <c r="J34" t="s">
         <v>367</v>
       </c>
-      <c r="C34" t="s">
+      <c r="K34" t="s">
+        <v>206</v>
+      </c>
+      <c r="L34" t="s">
+        <v>300</v>
+      </c>
+      <c r="M34" t="s">
         <v>368</v>
       </c>
-      <c r="D34" t="s">
+      <c r="P34" t="s">
         <v>369</v>
       </c>
-      <c r="E34" t="s">
+      <c r="Q34" t="s">
+        <v>115</v>
+      </c>
+      <c r="R34" t="s">
+        <v>27</v>
+      </c>
+      <c r="S34" t="s">
+        <v>27</v>
+      </c>
+      <c r="T34" t="s">
         <v>370</v>
       </c>
-      <c r="F34" t="s">
+      <c r="U34" t="s">
         <v>371</v>
       </c>
-      <c r="G34" t="s">
-        <v>222</v>
-      </c>
-      <c r="H34" t="s">
+      <c r="V34" t="s">
         <v>372</v>
-      </c>
-      <c r="I34" t="s">
-        <v>373</v>
-      </c>
-      <c r="J34" t="s">
-        <v>374</v>
-      </c>
-      <c r="K34" t="s">
-        <v>213</v>
-      </c>
-      <c r="L34" t="s">
-        <v>307</v>
-      </c>
-      <c r="M34" t="s">
-        <v>375</v>
-      </c>
-      <c r="P34" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>120</v>
-      </c>
-      <c r="R34" t="s">
-        <v>28</v>
-      </c>
-      <c r="S34" t="s">
-        <v>28</v>
-      </c>
-      <c r="T34" t="s">
-        <v>377</v>
-      </c>
-      <c r="U34" t="s">
-        <v>378</v>
-      </c>
-      <c r="V34" t="s">
-        <v>379</v>
       </c>
       <c r="W34">
         <v>0</v>
@@ -4039,64 +4053,64 @@
         <v>31858</v>
       </c>
       <c r="B35" t="s">
+        <v>373</v>
+      </c>
+      <c r="C35" t="s">
+        <v>374</v>
+      </c>
+      <c r="D35" t="s">
+        <v>375</v>
+      </c>
+      <c r="E35" t="s">
+        <v>376</v>
+      </c>
+      <c r="F35" t="s">
+        <v>377</v>
+      </c>
+      <c r="G35" t="s">
+        <v>378</v>
+      </c>
+      <c r="H35" t="s">
+        <v>379</v>
+      </c>
+      <c r="I35" t="s">
         <v>380</v>
       </c>
-      <c r="C35" t="s">
+      <c r="J35" t="s">
         <v>381</v>
       </c>
-      <c r="D35" t="s">
+      <c r="K35" t="s">
         <v>382</v>
       </c>
-      <c r="E35" t="s">
+      <c r="L35" t="s">
+        <v>26</v>
+      </c>
+      <c r="M35" t="s">
         <v>383</v>
       </c>
-      <c r="F35" t="s">
+      <c r="O35" t="s">
         <v>384</v>
       </c>
-      <c r="G35" t="s">
+      <c r="P35" t="s">
         <v>385</v>
       </c>
-      <c r="H35" t="s">
+      <c r="Q35" t="s">
         <v>386</v>
       </c>
-      <c r="I35" t="s">
+      <c r="R35" t="s">
+        <v>155</v>
+      </c>
+      <c r="S35" t="s">
         <v>387</v>
       </c>
-      <c r="J35" t="s">
+      <c r="T35" t="s">
+        <v>42</v>
+      </c>
+      <c r="U35" t="s">
         <v>388</v>
       </c>
-      <c r="K35" t="s">
+      <c r="V35" t="s">
         <v>389</v>
-      </c>
-      <c r="L35" t="s">
-        <v>27</v>
-      </c>
-      <c r="M35" t="s">
-        <v>390</v>
-      </c>
-      <c r="O35" t="s">
-        <v>391</v>
-      </c>
-      <c r="P35" t="s">
-        <v>392</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>393</v>
-      </c>
-      <c r="R35" t="s">
-        <v>161</v>
-      </c>
-      <c r="S35" t="s">
-        <v>394</v>
-      </c>
-      <c r="T35" t="s">
-        <v>43</v>
-      </c>
-      <c r="U35" t="s">
-        <v>395</v>
-      </c>
-      <c r="V35" t="s">
-        <v>396</v>
       </c>
       <c r="W35">
         <v>0</v>
@@ -4107,58 +4121,58 @@
         <v>33046</v>
       </c>
       <c r="B36" t="s">
+        <v>390</v>
+      </c>
+      <c r="C36" t="s">
+        <v>391</v>
+      </c>
+      <c r="E36" t="s">
+        <v>392</v>
+      </c>
+      <c r="F36" t="s">
+        <v>393</v>
+      </c>
+      <c r="G36" t="s">
+        <v>394</v>
+      </c>
+      <c r="H36" t="s">
+        <v>395</v>
+      </c>
+      <c r="I36" t="s">
+        <v>396</v>
+      </c>
+      <c r="J36" t="s">
         <v>397</v>
       </c>
-      <c r="C36" t="s">
+      <c r="K36" t="s">
+        <v>206</v>
+      </c>
+      <c r="L36" t="s">
+        <v>36</v>
+      </c>
+      <c r="M36" t="s">
         <v>398</v>
       </c>
-      <c r="E36" t="s">
+      <c r="P36" t="s">
         <v>399</v>
       </c>
-      <c r="F36" t="s">
+      <c r="Q36" t="s">
         <v>400</v>
       </c>
-      <c r="G36" t="s">
+      <c r="R36" t="s">
+        <v>220</v>
+      </c>
+      <c r="S36" t="s">
+        <v>221</v>
+      </c>
+      <c r="T36" t="s">
+        <v>222</v>
+      </c>
+      <c r="U36" t="s">
         <v>401</v>
       </c>
-      <c r="H36" t="s">
+      <c r="V36" t="s">
         <v>402</v>
-      </c>
-      <c r="I36" t="s">
-        <v>403</v>
-      </c>
-      <c r="J36" t="s">
-        <v>404</v>
-      </c>
-      <c r="K36" t="s">
-        <v>213</v>
-      </c>
-      <c r="L36" t="s">
-        <v>37</v>
-      </c>
-      <c r="M36" t="s">
-        <v>405</v>
-      </c>
-      <c r="P36" t="s">
-        <v>406</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>407</v>
-      </c>
-      <c r="R36" t="s">
-        <v>227</v>
-      </c>
-      <c r="S36" t="s">
-        <v>228</v>
-      </c>
-      <c r="T36" t="s">
-        <v>229</v>
-      </c>
-      <c r="U36" t="s">
-        <v>408</v>
-      </c>
-      <c r="V36" t="s">
-        <v>409</v>
       </c>
       <c r="W36">
         <v>0</v>
@@ -4169,58 +4183,58 @@
         <v>36559</v>
       </c>
       <c r="B37" t="s">
+        <v>403</v>
+      </c>
+      <c r="C37" t="s">
+        <v>404</v>
+      </c>
+      <c r="E37" t="s">
+        <v>405</v>
+      </c>
+      <c r="F37" t="s">
+        <v>348</v>
+      </c>
+      <c r="G37" t="s">
+        <v>348</v>
+      </c>
+      <c r="H37" t="s">
+        <v>406</v>
+      </c>
+      <c r="I37" t="s">
+        <v>407</v>
+      </c>
+      <c r="L37" t="s">
+        <v>233</v>
+      </c>
+      <c r="M37" t="s">
+        <v>408</v>
+      </c>
+      <c r="N37" t="s">
+        <v>409</v>
+      </c>
+      <c r="O37" t="s">
         <v>410</v>
       </c>
-      <c r="C37" t="s">
+      <c r="P37" t="s">
         <v>411</v>
       </c>
-      <c r="E37" t="s">
+      <c r="Q37" t="s">
+        <v>115</v>
+      </c>
+      <c r="R37" t="s">
+        <v>355</v>
+      </c>
+      <c r="S37" t="s">
         <v>412</v>
       </c>
-      <c r="F37" t="s">
-        <v>355</v>
-      </c>
-      <c r="G37" t="s">
-        <v>355</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="T37" t="s">
+        <v>357</v>
+      </c>
+      <c r="U37" t="s">
         <v>413</v>
       </c>
-      <c r="I37" t="s">
+      <c r="V37" t="s">
         <v>414</v>
-      </c>
-      <c r="L37" t="s">
-        <v>240</v>
-      </c>
-      <c r="M37" t="s">
-        <v>415</v>
-      </c>
-      <c r="N37" t="s">
-        <v>416</v>
-      </c>
-      <c r="O37" t="s">
-        <v>417</v>
-      </c>
-      <c r="P37" t="s">
-        <v>418</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>120</v>
-      </c>
-      <c r="R37" t="s">
-        <v>362</v>
-      </c>
-      <c r="S37" t="s">
-        <v>419</v>
-      </c>
-      <c r="T37" t="s">
-        <v>364</v>
-      </c>
-      <c r="U37" t="s">
-        <v>420</v>
-      </c>
-      <c r="V37" t="s">
-        <v>421</v>
       </c>
       <c r="W37">
         <v>0</v>
@@ -4231,55 +4245,55 @@
         <v>4394</v>
       </c>
       <c r="B38" t="s">
+        <v>415</v>
+      </c>
+      <c r="C38" t="s">
+        <v>416</v>
+      </c>
+      <c r="E38" t="s">
+        <v>417</v>
+      </c>
+      <c r="F38" t="s">
+        <v>418</v>
+      </c>
+      <c r="G38" t="s">
+        <v>419</v>
+      </c>
+      <c r="H38" t="s">
+        <v>420</v>
+      </c>
+      <c r="I38" t="s">
+        <v>421</v>
+      </c>
+      <c r="J38" t="s">
         <v>422</v>
       </c>
-      <c r="C38" t="s">
+      <c r="K38" t="s">
         <v>423</v>
       </c>
-      <c r="E38" t="s">
+      <c r="L38" t="s">
+        <v>36</v>
+      </c>
+      <c r="M38" t="s">
         <v>424</v>
       </c>
-      <c r="F38" t="s">
+      <c r="P38" t="s">
         <v>425</v>
       </c>
-      <c r="G38" t="s">
+      <c r="R38" t="s">
+        <v>155</v>
+      </c>
+      <c r="S38" t="s">
         <v>426</v>
       </c>
-      <c r="H38" t="s">
+      <c r="T38" t="s">
+        <v>42</v>
+      </c>
+      <c r="U38" t="s">
         <v>427</v>
       </c>
-      <c r="I38" t="s">
+      <c r="V38" t="s">
         <v>428</v>
-      </c>
-      <c r="J38" t="s">
-        <v>429</v>
-      </c>
-      <c r="K38" t="s">
-        <v>430</v>
-      </c>
-      <c r="L38" t="s">
-        <v>37</v>
-      </c>
-      <c r="M38" t="s">
-        <v>431</v>
-      </c>
-      <c r="P38" t="s">
-        <v>432</v>
-      </c>
-      <c r="R38" t="s">
-        <v>161</v>
-      </c>
-      <c r="S38" t="s">
-        <v>433</v>
-      </c>
-      <c r="T38" t="s">
-        <v>43</v>
-      </c>
-      <c r="U38" t="s">
-        <v>434</v>
-      </c>
-      <c r="V38" t="s">
-        <v>435</v>
       </c>
       <c r="W38">
         <v>0</v>
@@ -4290,64 +4304,64 @@
         <v>53327</v>
       </c>
       <c r="B39" t="s">
+        <v>429</v>
+      </c>
+      <c r="C39" t="s">
+        <v>430</v>
+      </c>
+      <c r="D39" t="s">
+        <v>431</v>
+      </c>
+      <c r="E39" t="s">
+        <v>432</v>
+      </c>
+      <c r="F39" t="s">
+        <v>433</v>
+      </c>
+      <c r="G39" t="s">
+        <v>434</v>
+      </c>
+      <c r="H39" t="s">
+        <v>151</v>
+      </c>
+      <c r="I39" t="s">
+        <v>435</v>
+      </c>
+      <c r="J39" t="s">
         <v>436</v>
       </c>
-      <c r="C39" t="s">
+      <c r="K39" t="s">
+        <v>153</v>
+      </c>
+      <c r="L39" t="s">
+        <v>36</v>
+      </c>
+      <c r="M39" t="s">
         <v>437</v>
       </c>
-      <c r="D39" t="s">
+      <c r="N39" t="s">
         <v>438</v>
       </c>
-      <c r="E39" t="s">
+      <c r="P39" t="s">
         <v>439</v>
       </c>
-      <c r="F39" t="s">
+      <c r="Q39" t="s">
+        <v>400</v>
+      </c>
+      <c r="R39" t="s">
+        <v>40</v>
+      </c>
+      <c r="S39" t="s">
         <v>440</v>
       </c>
-      <c r="G39" t="s">
+      <c r="T39" t="s">
+        <v>42</v>
+      </c>
+      <c r="U39" t="s">
         <v>441</v>
       </c>
-      <c r="H39" t="s">
-        <v>157</v>
-      </c>
-      <c r="I39" t="s">
+      <c r="V39" t="s">
         <v>442</v>
-      </c>
-      <c r="J39" t="s">
-        <v>443</v>
-      </c>
-      <c r="K39" t="s">
-        <v>159</v>
-      </c>
-      <c r="L39" t="s">
-        <v>37</v>
-      </c>
-      <c r="M39" t="s">
-        <v>444</v>
-      </c>
-      <c r="N39" t="s">
-        <v>445</v>
-      </c>
-      <c r="P39" t="s">
-        <v>446</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>407</v>
-      </c>
-      <c r="R39" t="s">
-        <v>41</v>
-      </c>
-      <c r="S39" t="s">
-        <v>447</v>
-      </c>
-      <c r="T39" t="s">
-        <v>43</v>
-      </c>
-      <c r="U39" t="s">
-        <v>448</v>
-      </c>
-      <c r="V39" t="s">
-        <v>449</v>
       </c>
       <c r="W39">
         <v>0</v>
@@ -4358,49 +4372,49 @@
         <v>54379</v>
       </c>
       <c r="B40" t="s">
+        <v>443</v>
+      </c>
+      <c r="C40" t="s">
+        <v>444</v>
+      </c>
+      <c r="D40" t="s">
+        <v>445</v>
+      </c>
+      <c r="E40" t="s">
+        <v>446</v>
+      </c>
+      <c r="F40" t="s">
+        <v>447</v>
+      </c>
+      <c r="G40" t="s">
+        <v>448</v>
+      </c>
+      <c r="H40" t="s">
+        <v>153</v>
+      </c>
+      <c r="I40" t="s">
+        <v>449</v>
+      </c>
+      <c r="L40" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>400</v>
+      </c>
+      <c r="R40" t="s">
+        <v>155</v>
+      </c>
+      <c r="S40" t="s">
+        <v>426</v>
+      </c>
+      <c r="T40" t="s">
+        <v>42</v>
+      </c>
+      <c r="U40" t="s">
         <v>450</v>
       </c>
-      <c r="C40" t="s">
+      <c r="V40" t="s">
         <v>451</v>
-      </c>
-      <c r="D40" t="s">
-        <v>452</v>
-      </c>
-      <c r="E40" t="s">
-        <v>453</v>
-      </c>
-      <c r="F40" t="s">
-        <v>454</v>
-      </c>
-      <c r="G40" t="s">
-        <v>455</v>
-      </c>
-      <c r="H40" t="s">
-        <v>159</v>
-      </c>
-      <c r="I40" t="s">
-        <v>456</v>
-      </c>
-      <c r="L40" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>407</v>
-      </c>
-      <c r="R40" t="s">
-        <v>161</v>
-      </c>
-      <c r="S40" t="s">
-        <v>433</v>
-      </c>
-      <c r="T40" t="s">
-        <v>43</v>
-      </c>
-      <c r="U40" t="s">
-        <v>457</v>
-      </c>
-      <c r="V40" t="s">
-        <v>458</v>
       </c>
       <c r="W40">
         <v>0</v>
@@ -4411,55 +4425,55 @@
         <v>64491</v>
       </c>
       <c r="B41" t="s">
+        <v>452</v>
+      </c>
+      <c r="C41" t="s">
+        <v>453</v>
+      </c>
+      <c r="E41" t="s">
+        <v>454</v>
+      </c>
+      <c r="F41" t="s">
+        <v>455</v>
+      </c>
+      <c r="G41" t="s">
+        <v>456</v>
+      </c>
+      <c r="H41" t="s">
+        <v>153</v>
+      </c>
+      <c r="I41" t="s">
+        <v>457</v>
+      </c>
+      <c r="L41" t="s">
+        <v>36</v>
+      </c>
+      <c r="M41" t="s">
+        <v>458</v>
+      </c>
+      <c r="O41" t="s">
         <v>459</v>
       </c>
-      <c r="C41" t="s">
+      <c r="P41" t="s">
         <v>460</v>
       </c>
-      <c r="E41" t="s">
+      <c r="Q41" t="s">
+        <v>253</v>
+      </c>
+      <c r="R41" t="s">
+        <v>171</v>
+      </c>
+      <c r="S41" t="s">
         <v>461</v>
       </c>
-      <c r="F41" t="s">
+      <c r="T41" t="s">
+        <v>42</v>
+      </c>
+      <c r="U41" t="s">
         <v>462</v>
       </c>
-      <c r="G41" t="s">
+      <c r="V41" t="s">
         <v>463</v>
-      </c>
-      <c r="H41" t="s">
-        <v>159</v>
-      </c>
-      <c r="I41" t="s">
-        <v>464</v>
-      </c>
-      <c r="L41" t="s">
-        <v>37</v>
-      </c>
-      <c r="M41" t="s">
-        <v>465</v>
-      </c>
-      <c r="O41" t="s">
-        <v>466</v>
-      </c>
-      <c r="P41" t="s">
-        <v>467</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>260</v>
-      </c>
-      <c r="R41" t="s">
-        <v>178</v>
-      </c>
-      <c r="S41" t="s">
-        <v>468</v>
-      </c>
-      <c r="T41" t="s">
-        <v>43</v>
-      </c>
-      <c r="U41" t="s">
-        <v>469</v>
-      </c>
-      <c r="V41" t="s">
-        <v>470</v>
       </c>
       <c r="W41">
         <v>0</v>
@@ -4470,43 +4484,43 @@
         <v>66020</v>
       </c>
       <c r="B42" t="s">
+        <v>464</v>
+      </c>
+      <c r="C42" t="s">
+        <v>465</v>
+      </c>
+      <c r="E42" t="s">
+        <v>466</v>
+      </c>
+      <c r="F42" t="s">
+        <v>467</v>
+      </c>
+      <c r="G42" t="s">
+        <v>468</v>
+      </c>
+      <c r="H42" t="s">
+        <v>469</v>
+      </c>
+      <c r="J42" t="s">
+        <v>470</v>
+      </c>
+      <c r="L42" t="s">
+        <v>233</v>
+      </c>
+      <c r="O42" t="s">
         <v>471</v>
       </c>
-      <c r="C42" t="s">
+      <c r="R42" t="s">
+        <v>27</v>
+      </c>
+      <c r="S42" t="s">
+        <v>27</v>
+      </c>
+      <c r="U42" t="s">
         <v>472</v>
       </c>
-      <c r="E42" t="s">
+      <c r="V42" t="s">
         <v>473</v>
-      </c>
-      <c r="F42" t="s">
-        <v>474</v>
-      </c>
-      <c r="G42" t="s">
-        <v>475</v>
-      </c>
-      <c r="H42" t="s">
-        <v>476</v>
-      </c>
-      <c r="J42" t="s">
-        <v>477</v>
-      </c>
-      <c r="L42" t="s">
-        <v>240</v>
-      </c>
-      <c r="O42" t="s">
-        <v>478</v>
-      </c>
-      <c r="R42" t="s">
-        <v>28</v>
-      </c>
-      <c r="S42" t="s">
-        <v>28</v>
-      </c>
-      <c r="U42" t="s">
-        <v>479</v>
-      </c>
-      <c r="V42" t="s">
-        <v>480</v>
       </c>
       <c r="W42">
         <v>0</v>
@@ -4517,58 +4531,58 @@
         <v>68789</v>
       </c>
       <c r="B43" t="s">
+        <v>474</v>
+      </c>
+      <c r="C43" t="s">
+        <v>475</v>
+      </c>
+      <c r="D43" t="s">
+        <v>476</v>
+      </c>
+      <c r="E43" t="s">
+        <v>477</v>
+      </c>
+      <c r="F43" t="s">
+        <v>478</v>
+      </c>
+      <c r="G43" t="s">
+        <v>24</v>
+      </c>
+      <c r="H43" t="s">
+        <v>206</v>
+      </c>
+      <c r="I43" t="s">
+        <v>479</v>
+      </c>
+      <c r="K43" t="s">
+        <v>206</v>
+      </c>
+      <c r="L43" t="s">
+        <v>26</v>
+      </c>
+      <c r="M43" t="s">
+        <v>480</v>
+      </c>
+      <c r="P43" t="s">
         <v>481</v>
       </c>
-      <c r="C43" t="s">
+      <c r="Q43" t="s">
+        <v>253</v>
+      </c>
+      <c r="R43" t="s">
+        <v>27</v>
+      </c>
+      <c r="S43" t="s">
+        <v>27</v>
+      </c>
+      <c r="T43" t="s">
         <v>482</v>
       </c>
-      <c r="D43" t="s">
+      <c r="U43" t="s">
         <v>483</v>
       </c>
-      <c r="E43" t="s">
+      <c r="V43" t="s">
         <v>484</v>
-      </c>
-      <c r="F43" t="s">
-        <v>485</v>
-      </c>
-      <c r="G43" t="s">
-        <v>25</v>
-      </c>
-      <c r="H43" t="s">
-        <v>213</v>
-      </c>
-      <c r="I43" t="s">
-        <v>486</v>
-      </c>
-      <c r="K43" t="s">
-        <v>213</v>
-      </c>
-      <c r="L43" t="s">
-        <v>27</v>
-      </c>
-      <c r="M43" t="s">
-        <v>487</v>
-      </c>
-      <c r="P43" t="s">
-        <v>488</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>260</v>
-      </c>
-      <c r="R43" t="s">
-        <v>28</v>
-      </c>
-      <c r="S43" t="s">
-        <v>28</v>
-      </c>
-      <c r="T43" t="s">
-        <v>489</v>
-      </c>
-      <c r="U43" t="s">
-        <v>490</v>
-      </c>
-      <c r="V43" t="s">
-        <v>491</v>
       </c>
       <c r="W43">
         <v>0</v>
@@ -4579,40 +4593,40 @@
         <v>7200000021</v>
       </c>
       <c r="B44" t="s">
+        <v>485</v>
+      </c>
+      <c r="C44" t="s">
+        <v>486</v>
+      </c>
+      <c r="E44" t="s">
+        <v>487</v>
+      </c>
+      <c r="F44" t="s">
+        <v>488</v>
+      </c>
+      <c r="G44" t="s">
+        <v>488</v>
+      </c>
+      <c r="I44" t="s">
+        <v>489</v>
+      </c>
+      <c r="L44" t="s">
+        <v>490</v>
+      </c>
+      <c r="R44" t="s">
+        <v>171</v>
+      </c>
+      <c r="S44" t="s">
+        <v>172</v>
+      </c>
+      <c r="T44" t="s">
+        <v>173</v>
+      </c>
+      <c r="U44" t="s">
+        <v>491</v>
+      </c>
+      <c r="V44" t="s">
         <v>492</v>
-      </c>
-      <c r="C44" t="s">
-        <v>493</v>
-      </c>
-      <c r="E44" t="s">
-        <v>494</v>
-      </c>
-      <c r="F44" t="s">
-        <v>495</v>
-      </c>
-      <c r="G44" t="s">
-        <v>495</v>
-      </c>
-      <c r="I44" t="s">
-        <v>496</v>
-      </c>
-      <c r="L44" t="s">
-        <v>497</v>
-      </c>
-      <c r="R44" t="s">
-        <v>178</v>
-      </c>
-      <c r="S44" t="s">
-        <v>179</v>
-      </c>
-      <c r="T44" t="s">
-        <v>180</v>
-      </c>
-      <c r="U44" t="s">
-        <v>498</v>
-      </c>
-      <c r="V44" t="s">
-        <v>499</v>
       </c>
       <c r="W44">
         <v>0</v>
@@ -4623,55 +4637,55 @@
         <v>76630</v>
       </c>
       <c r="B45" t="s">
+        <v>493</v>
+      </c>
+      <c r="C45" t="s">
+        <v>494</v>
+      </c>
+      <c r="E45" t="s">
+        <v>495</v>
+      </c>
+      <c r="F45" t="s">
+        <v>496</v>
+      </c>
+      <c r="G45" t="s">
+        <v>497</v>
+      </c>
+      <c r="H45" t="s">
+        <v>151</v>
+      </c>
+      <c r="I45" t="s">
+        <v>498</v>
+      </c>
+      <c r="J45" t="s">
+        <v>100</v>
+      </c>
+      <c r="K45" t="s">
+        <v>153</v>
+      </c>
+      <c r="L45" t="s">
+        <v>36</v>
+      </c>
+      <c r="M45" t="s">
+        <v>499</v>
+      </c>
+      <c r="P45" t="s">
         <v>500</v>
       </c>
-      <c r="C45" t="s">
+      <c r="R45" t="s">
+        <v>155</v>
+      </c>
+      <c r="S45" t="s">
+        <v>156</v>
+      </c>
+      <c r="T45" t="s">
+        <v>42</v>
+      </c>
+      <c r="U45" t="s">
         <v>501</v>
       </c>
-      <c r="E45" t="s">
+      <c r="V45" t="s">
         <v>502</v>
-      </c>
-      <c r="F45" t="s">
-        <v>503</v>
-      </c>
-      <c r="G45" t="s">
-        <v>504</v>
-      </c>
-      <c r="H45" t="s">
-        <v>157</v>
-      </c>
-      <c r="I45" t="s">
-        <v>505</v>
-      </c>
-      <c r="J45" t="s">
-        <v>104</v>
-      </c>
-      <c r="K45" t="s">
-        <v>159</v>
-      </c>
-      <c r="L45" t="s">
-        <v>37</v>
-      </c>
-      <c r="M45" t="s">
-        <v>506</v>
-      </c>
-      <c r="P45" t="s">
-        <v>507</v>
-      </c>
-      <c r="R45" t="s">
-        <v>161</v>
-      </c>
-      <c r="S45" t="s">
-        <v>162</v>
-      </c>
-      <c r="T45" t="s">
-        <v>43</v>
-      </c>
-      <c r="U45" t="s">
-        <v>508</v>
-      </c>
-      <c r="V45" t="s">
-        <v>509</v>
       </c>
       <c r="W45">
         <v>0</v>
@@ -4682,49 +4696,49 @@
         <v>79150</v>
       </c>
       <c r="B46" t="s">
+        <v>503</v>
+      </c>
+      <c r="C46" t="s">
+        <v>504</v>
+      </c>
+      <c r="E46" t="s">
+        <v>505</v>
+      </c>
+      <c r="F46" t="s">
+        <v>97</v>
+      </c>
+      <c r="G46" t="s">
+        <v>97</v>
+      </c>
+      <c r="H46" t="s">
+        <v>506</v>
+      </c>
+      <c r="I46" t="s">
+        <v>507</v>
+      </c>
+      <c r="L46" t="s">
+        <v>233</v>
+      </c>
+      <c r="O46" t="s">
+        <v>508</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>115</v>
+      </c>
+      <c r="R46" t="s">
+        <v>40</v>
+      </c>
+      <c r="S46" t="s">
+        <v>440</v>
+      </c>
+      <c r="T46" t="s">
+        <v>42</v>
+      </c>
+      <c r="U46" t="s">
+        <v>509</v>
+      </c>
+      <c r="V46" t="s">
         <v>510</v>
-      </c>
-      <c r="C46" t="s">
-        <v>511</v>
-      </c>
-      <c r="E46" t="s">
-        <v>512</v>
-      </c>
-      <c r="F46" t="s">
-        <v>101</v>
-      </c>
-      <c r="G46" t="s">
-        <v>101</v>
-      </c>
-      <c r="H46" t="s">
-        <v>513</v>
-      </c>
-      <c r="I46" t="s">
-        <v>514</v>
-      </c>
-      <c r="L46" t="s">
-        <v>240</v>
-      </c>
-      <c r="O46" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>120</v>
-      </c>
-      <c r="R46" t="s">
-        <v>41</v>
-      </c>
-      <c r="S46" t="s">
-        <v>447</v>
-      </c>
-      <c r="T46" t="s">
-        <v>43</v>
-      </c>
-      <c r="U46" t="s">
-        <v>516</v>
-      </c>
-      <c r="V46" t="s">
-        <v>517</v>
       </c>
       <c r="W46">
         <v>0</v>
@@ -4735,55 +4749,55 @@
         <v>8295616241</v>
       </c>
       <c r="B47" t="s">
+        <v>511</v>
+      </c>
+      <c r="C47" t="s">
+        <v>512</v>
+      </c>
+      <c r="E47" t="s">
+        <v>513</v>
+      </c>
+      <c r="F47" t="s">
+        <v>514</v>
+      </c>
+      <c r="G47" t="s">
+        <v>515</v>
+      </c>
+      <c r="H47" t="s">
+        <v>516</v>
+      </c>
+      <c r="I47" t="s">
+        <v>517</v>
+      </c>
+      <c r="J47" t="s">
+        <v>26</v>
+      </c>
+      <c r="L47" t="s">
+        <v>26</v>
+      </c>
+      <c r="M47" t="s">
         <v>518</v>
       </c>
-      <c r="C47" t="s">
+      <c r="O47" t="s">
+        <v>459</v>
+      </c>
+      <c r="P47" t="s">
         <v>519</v>
       </c>
-      <c r="E47" t="s">
+      <c r="R47" t="s">
+        <v>27</v>
+      </c>
+      <c r="S47" t="s">
+        <v>27</v>
+      </c>
+      <c r="T47" t="s">
+        <v>517</v>
+      </c>
+      <c r="U47" t="s">
         <v>520</v>
       </c>
-      <c r="F47" t="s">
+      <c r="V47" t="s">
         <v>521</v>
-      </c>
-      <c r="G47" t="s">
-        <v>522</v>
-      </c>
-      <c r="H47" t="s">
-        <v>523</v>
-      </c>
-      <c r="I47" t="s">
-        <v>524</v>
-      </c>
-      <c r="J47" t="s">
-        <v>27</v>
-      </c>
-      <c r="L47" t="s">
-        <v>27</v>
-      </c>
-      <c r="M47" t="s">
-        <v>525</v>
-      </c>
-      <c r="O47" t="s">
-        <v>466</v>
-      </c>
-      <c r="P47" t="s">
-        <v>526</v>
-      </c>
-      <c r="R47" t="s">
-        <v>28</v>
-      </c>
-      <c r="S47" t="s">
-        <v>28</v>
-      </c>
-      <c r="T47" t="s">
-        <v>524</v>
-      </c>
-      <c r="U47" t="s">
-        <v>527</v>
-      </c>
-      <c r="V47" t="s">
-        <v>528</v>
       </c>
       <c r="W47">
         <v>0</v>
@@ -4794,52 +4808,52 @@
         <v>88862</v>
       </c>
       <c r="B48" t="s">
+        <v>522</v>
+      </c>
+      <c r="C48" t="s">
+        <v>430</v>
+      </c>
+      <c r="E48" t="s">
+        <v>523</v>
+      </c>
+      <c r="F48" t="s">
+        <v>524</v>
+      </c>
+      <c r="G48" t="s">
+        <v>525</v>
+      </c>
+      <c r="H48" t="s">
+        <v>151</v>
+      </c>
+      <c r="I48" t="s">
+        <v>526</v>
+      </c>
+      <c r="L48" t="s">
+        <v>36</v>
+      </c>
+      <c r="M48" t="s">
+        <v>527</v>
+      </c>
+      <c r="P48" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>400</v>
+      </c>
+      <c r="R48" t="s">
+        <v>40</v>
+      </c>
+      <c r="S48" t="s">
+        <v>440</v>
+      </c>
+      <c r="T48" t="s">
+        <v>42</v>
+      </c>
+      <c r="U48" t="s">
+        <v>528</v>
+      </c>
+      <c r="V48" t="s">
         <v>529</v>
-      </c>
-      <c r="C48" t="s">
-        <v>437</v>
-      </c>
-      <c r="E48" t="s">
-        <v>530</v>
-      </c>
-      <c r="F48" t="s">
-        <v>531</v>
-      </c>
-      <c r="G48" t="s">
-        <v>532</v>
-      </c>
-      <c r="H48" t="s">
-        <v>157</v>
-      </c>
-      <c r="I48" t="s">
-        <v>533</v>
-      </c>
-      <c r="L48" t="s">
-        <v>37</v>
-      </c>
-      <c r="M48" t="s">
-        <v>534</v>
-      </c>
-      <c r="P48" t="s">
-        <v>446</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>407</v>
-      </c>
-      <c r="R48" t="s">
-        <v>41</v>
-      </c>
-      <c r="S48" t="s">
-        <v>447</v>
-      </c>
-      <c r="T48" t="s">
-        <v>43</v>
-      </c>
-      <c r="U48" t="s">
-        <v>535</v>
-      </c>
-      <c r="V48" t="s">
-        <v>536</v>
       </c>
       <c r="W48">
         <v>0</v>
@@ -4850,67 +4864,67 @@
         <v>90100</v>
       </c>
       <c r="B49" t="s">
+        <v>530</v>
+      </c>
+      <c r="C49" t="s">
+        <v>531</v>
+      </c>
+      <c r="D49" t="s">
+        <v>532</v>
+      </c>
+      <c r="E49" t="s">
+        <v>533</v>
+      </c>
+      <c r="F49" t="s">
+        <v>534</v>
+      </c>
+      <c r="G49" t="s">
+        <v>535</v>
+      </c>
+      <c r="H49" t="s">
+        <v>365</v>
+      </c>
+      <c r="I49" t="s">
+        <v>536</v>
+      </c>
+      <c r="J49" t="s">
+        <v>26</v>
+      </c>
+      <c r="K49" t="s">
+        <v>206</v>
+      </c>
+      <c r="L49" t="s">
+        <v>26</v>
+      </c>
+      <c r="M49" t="s">
         <v>537</v>
       </c>
-      <c r="C49" t="s">
+      <c r="N49" t="s">
         <v>538</v>
       </c>
-      <c r="D49" t="s">
+      <c r="O49" t="s">
+        <v>533</v>
+      </c>
+      <c r="P49" t="s">
         <v>539</v>
       </c>
-      <c r="E49" t="s">
+      <c r="Q49" t="s">
+        <v>400</v>
+      </c>
+      <c r="R49" t="s">
+        <v>355</v>
+      </c>
+      <c r="S49" t="s">
+        <v>412</v>
+      </c>
+      <c r="T49" t="s">
+        <v>357</v>
+      </c>
+      <c r="U49" t="s">
         <v>540</v>
       </c>
-      <c r="F49" t="s">
+      <c r="V49" t="s">
         <v>541</v>
-      </c>
-      <c r="G49" t="s">
-        <v>542</v>
-      </c>
-      <c r="H49" t="s">
-        <v>372</v>
-      </c>
-      <c r="I49" t="s">
-        <v>543</v>
-      </c>
-      <c r="J49" t="s">
-        <v>27</v>
-      </c>
-      <c r="K49" t="s">
-        <v>213</v>
-      </c>
-      <c r="L49" t="s">
-        <v>27</v>
-      </c>
-      <c r="M49" t="s">
-        <v>544</v>
-      </c>
-      <c r="N49" t="s">
-        <v>545</v>
-      </c>
-      <c r="O49" t="s">
-        <v>540</v>
-      </c>
-      <c r="P49" t="s">
-        <v>546</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>407</v>
-      </c>
-      <c r="R49" t="s">
-        <v>362</v>
-      </c>
-      <c r="S49" t="s">
-        <v>419</v>
-      </c>
-      <c r="T49" t="s">
-        <v>364</v>
-      </c>
-      <c r="U49" t="s">
-        <v>547</v>
-      </c>
-      <c r="V49" t="s">
-        <v>548</v>
       </c>
       <c r="W49">
         <v>0</v>
@@ -4921,49 +4935,49 @@
         <v>9138378043</v>
       </c>
       <c r="B50" t="s">
+        <v>542</v>
+      </c>
+      <c r="C50" t="s">
+        <v>543</v>
+      </c>
+      <c r="E50" t="s">
+        <v>544</v>
+      </c>
+      <c r="F50" t="s">
+        <v>545</v>
+      </c>
+      <c r="G50" t="s">
+        <v>97</v>
+      </c>
+      <c r="I50" t="s">
+        <v>546</v>
+      </c>
+      <c r="J50" t="s">
+        <v>470</v>
+      </c>
+      <c r="L50" t="s">
+        <v>233</v>
+      </c>
+      <c r="M50" t="s">
+        <v>547</v>
+      </c>
+      <c r="P50" t="s">
+        <v>548</v>
+      </c>
+      <c r="R50" t="s">
+        <v>66</v>
+      </c>
+      <c r="S50" t="s">
+        <v>234</v>
+      </c>
+      <c r="T50" t="s">
+        <v>66</v>
+      </c>
+      <c r="U50" t="s">
         <v>549</v>
       </c>
-      <c r="C50" t="s">
+      <c r="V50" t="s">
         <v>550</v>
-      </c>
-      <c r="E50" t="s">
-        <v>551</v>
-      </c>
-      <c r="F50" t="s">
-        <v>552</v>
-      </c>
-      <c r="G50" t="s">
-        <v>101</v>
-      </c>
-      <c r="I50" t="s">
-        <v>553</v>
-      </c>
-      <c r="J50" t="s">
-        <v>477</v>
-      </c>
-      <c r="L50" t="s">
-        <v>240</v>
-      </c>
-      <c r="M50" t="s">
-        <v>554</v>
-      </c>
-      <c r="P50" t="s">
-        <v>555</v>
-      </c>
-      <c r="R50" t="s">
-        <v>69</v>
-      </c>
-      <c r="S50" t="s">
-        <v>241</v>
-      </c>
-      <c r="T50" t="s">
-        <v>69</v>
-      </c>
-      <c r="U50" t="s">
-        <v>556</v>
-      </c>
-      <c r="V50" t="s">
-        <v>557</v>
       </c>
       <c r="W50">
         <v>0</v>
@@ -4974,58 +4988,58 @@
         <v>9300003346</v>
       </c>
       <c r="B51" t="s">
+        <v>551</v>
+      </c>
+      <c r="C51" t="s">
+        <v>552</v>
+      </c>
+      <c r="E51" t="s">
+        <v>553</v>
+      </c>
+      <c r="F51" t="s">
+        <v>554</v>
+      </c>
+      <c r="G51" t="s">
+        <v>555</v>
+      </c>
+      <c r="H51" t="s">
+        <v>556</v>
+      </c>
+      <c r="I51" t="s">
+        <v>557</v>
+      </c>
+      <c r="J51" t="s">
         <v>558</v>
       </c>
-      <c r="C51" t="s">
+      <c r="K51" t="s">
         <v>559</v>
       </c>
-      <c r="E51" t="s">
+      <c r="L51" t="s">
+        <v>233</v>
+      </c>
+      <c r="M51" t="s">
         <v>560</v>
       </c>
-      <c r="F51" t="s">
+      <c r="O51" t="s">
         <v>561</v>
       </c>
-      <c r="G51" t="s">
+      <c r="P51" t="s">
         <v>562</v>
       </c>
-      <c r="H51" t="s">
+      <c r="R51" t="s">
+        <v>27</v>
+      </c>
+      <c r="S51" t="s">
+        <v>27</v>
+      </c>
+      <c r="T51" t="s">
+        <v>557</v>
+      </c>
+      <c r="U51" t="s">
         <v>563</v>
       </c>
-      <c r="I51" t="s">
+      <c r="V51" t="s">
         <v>564</v>
-      </c>
-      <c r="J51" t="s">
-        <v>565</v>
-      </c>
-      <c r="K51" t="s">
-        <v>566</v>
-      </c>
-      <c r="L51" t="s">
-        <v>240</v>
-      </c>
-      <c r="M51" t="s">
-        <v>567</v>
-      </c>
-      <c r="O51" t="s">
-        <v>568</v>
-      </c>
-      <c r="P51" t="s">
-        <v>569</v>
-      </c>
-      <c r="R51" t="s">
-        <v>28</v>
-      </c>
-      <c r="S51" t="s">
-        <v>28</v>
-      </c>
-      <c r="T51" t="s">
-        <v>564</v>
-      </c>
-      <c r="U51" t="s">
-        <v>570</v>
-      </c>
-      <c r="V51" t="s">
-        <v>571</v>
       </c>
       <c r="W51">
         <v>0</v>

</xml_diff>